<commit_message>
introduction paragraph thesis structure
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880389EC-1EAE-E84E-8949-6A7E08270ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D440DE92-376C-6D49-BE33-C3DD7185AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -201,9 +201,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -220,6 +217,9 @@
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,11 +552,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
     </row>
     <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -584,13 +584,13 @@
       <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -617,7 +617,7 @@
       <c r="I3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K3" s="4" t="s">
@@ -650,7 +650,7 @@
       <c r="I4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K4" s="4" t="s">
@@ -683,7 +683,7 @@
       <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K5" s="4" t="s">
@@ -814,35 +814,35 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="D10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="9">
         <v>24000</v>
       </c>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10">
+      <c r="F10" s="9"/>
+      <c r="G10" s="9">
         <v>33392</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="9">
         <v>16007</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <f>1-H10/G10</f>
         <v>0.52063368471490179</v>
       </c>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C11" s="4"/>

</xml_diff>

<commit_message>
done more experiments on matmul, starting to better understand the optimizations' behavior
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D440DE92-376C-6D49-BE33-C3DD7185AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{138A5786-6247-6C41-9751-C9B63BACAF62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>selected code</t>
   </si>
@@ -143,6 +143,122 @@
                                           output/01searched-edited.mlir \
                                           -o output/04optimized.mlir \
                                           2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                       soda-opt \
+                                                         -soda-outline-bambu-code \
+                                                         -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                         -soda-generate-bambu-accelcode \
+                                                         --convert-linalg-to-affine-loops \
+                                                         -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                         -mlir-print-ir-after-all \
+                                                         output/01searched-edited.mlir \
+                                                         -o output/04optimized.mlir \
+                                                         2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir </t>
+  </si>
+  <si>
+    <t>Simple execution with no optimization. The only pass is a lower of the affine. I was not expecting any change in the number of cycles, instead I obtained the same number of cycles of the same command with the full unroll. By loogin at the dot graphs I noticed that the most inner loop disappeared, probably due to some optimizations made by clang. This explain the reduction of the number of cycles.</t>
+  </si>
+  <si>
+    <t>2 loops, I noticed a lot of mul in parallel, but few load.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                       soda-opt \
+                                                         -soda-outline-bambu-code \
+                                                         -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                         -soda-generate-bambu-accelcode \
+                                                         --convert-linalg-to-affine-loops \
+                                                         --affine-loop-unroll="unroll-full" \
+                                                         -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                         -mlir-print-ir-after-all \
+                                                         output/01searched-edited.mlir \
+                                                         -o output/04optimized.mlir \
+                                                         2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>Added the loop optimization, little change from the command above, equal to the full unroll 1 as expected</t>
+  </si>
+  <si>
+    <t>Added two full unrolls, exptected the same behaviour of the optimized with two full unrolls</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                       soda-opt \
+                                                         -soda-outline-bambu-code \
+                                                         -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                         -soda-generate-bambu-accelcode \
+                                                         --convert-linalg-to-affine-loops \
+                                                         --affine-loop-unroll="unroll-full" \   
+                                                         --affine-loop-unroll="unroll-full" \                                                             
+                                                         -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                         -mlir-print-ir-after-all \
+                                                         output/01searched-edited.mlir \
+                                                         -o output/04optimized.mlir \
+                                                         2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                       soda-opt \
+                                                         -soda-outline-bambu-code \
+                                                         -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                         -soda-generate-bambu-accelcode \
+                                                         --convert-linalg-to-affine-loops \
+                                                         --affine-loop-unroll="unroll-full" \   
+                                                         --affine-loop-unroll="unroll-full" \      
+                                                         --affine-loop-unroll="unroll-full"\                                                                                                                    
+                                                         -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                         -mlir-print-ir-after-all \
+                                                         output/01searched-edited.mlir \
+                                                         -o output/04optimized.mlir \
+                                                         2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>3 full loops unroll</t>
+  </si>
+  <si>
+    <t>%Error: Verilator threw signal 9.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                       soda-opt \
+                                                         -soda-outline-bambu-code \
+                                                         -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                         -soda-generate-bambu-accelcode \
+                                                         --convert-linalg-to-affine-loops \
+                                                         --affine-loop-unroll="unroll-num-reps=10" \
+                                                         -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                         -mlir-print-ir-after-all \
+                                                         output/01searched-edited.mlir \
+                                                         -o output/04optimized.mlir \
+                                                         2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>unroll the innermost loop repeadetly 10 times, the expectation is to have a slightly recutrion in the number of cycles, but it is not the case. The dot file seems to be equal to the one full unroll, even num-reps=100 had no effect. The idea is to repeat it two times, it probably has no effect because the innermost loop is unrolled in lower steps. This idea had no effect, still same number of cycles.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                       soda-opt \
+                                                         -soda-outline-bambu-code \
+                                                         -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                         -soda-generate-bambu-accelcode \
+                                                         --convert-linalg-to-affine-loops \
+                                                         --affine-loop-unroll="unroll-full" \
+                                                         --affine-loop-unroll="unroll-num-reps=1" \
+                                                         -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                         -mlir-print-ir-after-all \
+                                                         output/01searched-edited.mlir \
+                                                         -o output/04optimized.mlir \
+                                                         2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>I see always 2 loops, but the innermost is made of a big unrolled part and a small repeated part.</t>
+  </si>
+  <si>
+    <t>The idea here is to have the innermost cycle completely unrolled. While the second innermost loop is unrolled just one time. 
+This should return a number of cycles between the 16k of full unroll 1 and the 1k of 2 full unrolls. This theory is verified but not completely.
+I expect to have, since the two matrices are 15x15 and 15x16, three loops, of lenght (from the innermost one to the outermost) respectively 15, 16, 15.</t>
   </si>
 </sst>
 </file>
@@ -172,12 +288,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -192,7 +320,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -220,6 +348,26 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -535,275 +683,295 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="61.5" customWidth="1"/>
-    <col min="4" max="5" width="20.83203125" customWidth="1"/>
-    <col min="6" max="6" width="1.6640625" customWidth="1"/>
-    <col min="7" max="9" width="20.83203125" customWidth="1"/>
-    <col min="10" max="12" width="23.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="19" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="49.1640625" customWidth="1"/>
+    <col min="4" max="4" width="72.33203125" customWidth="1"/>
+    <col min="5" max="6" width="20.83203125" customWidth="1"/>
+    <col min="7" max="7" width="1.6640625" customWidth="1"/>
+    <col min="8" max="10" width="20.83203125" customWidth="1"/>
+    <col min="11" max="13" width="23.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="J1" s="11" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="11"/>
       <c r="L1" s="11"/>
-    </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="M1" s="11"/>
+    </row>
+    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A3" s="19">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="2">
+      <c r="F3" s="2">
         <v>434406528</v>
       </c>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="G3" s="2"/>
       <c r="H3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="I3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>22</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="M3" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" s="19">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="2">
+      <c r="F4" s="2">
         <v>434406528</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4" s="4" t="s">
+      <c r="I4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="M4" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="19">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="2">
+      <c r="F5" s="2">
         <v>434406528</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="G5" s="2"/>
       <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K5" s="4" t="s">
+      <c r="I5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="M5" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A6" s="19">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="2">
+      <c r="F6" s="2">
         <v>24000</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2">
-        <v>33392</v>
-      </c>
+      <c r="G6" s="2"/>
       <c r="H6" s="2">
         <v>33392</v>
       </c>
-      <c r="I6" s="3">
-        <f>1-H6/G6</f>
+      <c r="I6" s="2">
+        <v>33392</v>
+      </c>
+      <c r="J6" s="3">
+        <f>1-I6/H6</f>
         <v>0</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="19">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="2">
+      <c r="F7" s="2">
         <v>24000</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2">
         <v>33392</v>
       </c>
-      <c r="H7" s="2">
+      <c r="I7" s="17">
         <v>15992</v>
       </c>
-      <c r="I7" s="3">
-        <f>1-H7/G7</f>
+      <c r="J7" s="3">
+        <f>1-I7/H7</f>
         <v>0.52108289410637276</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="19">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="2">
+      <c r="F8" s="2">
         <v>24000</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2">
         <v>33392</v>
       </c>
-      <c r="H8" s="2">
+      <c r="I8" s="15">
         <v>1232</v>
       </c>
-      <c r="I8" s="3">
-        <f>1-H8/G8</f>
+      <c r="J8" s="3">
+        <f>1-I8/H8</f>
         <v>0.96310493531384767</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="K8" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="19">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2">
+      <c r="F9" s="2">
         <v>24000</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2">
+      <c r="G9" s="2"/>
+      <c r="H9" s="2">
         <v>33392</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="J9" s="4" t="s">
+      <c r="I9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>22</v>
       </c>
       <c r="K9" s="4" t="s">
@@ -812,282 +980,444 @@
       <c r="L9" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="409.6" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
+      <c r="M9" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="19">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="9">
+      <c r="F10" s="9">
         <v>24000</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9">
+      <c r="G10" s="9"/>
+      <c r="H10" s="9">
         <v>33392</v>
       </c>
-      <c r="H10" s="9">
+      <c r="I10" s="9">
         <v>16007</v>
       </c>
-      <c r="I10" s="10">
-        <f>1-H10/G10</f>
+      <c r="J10" s="10">
+        <f>1-I10/H10</f>
         <v>0.52063368471490179</v>
       </c>
-      <c r="J10" s="8"/>
       <c r="K10" s="8"/>
       <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C11" s="4"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C12" s="4"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C13" s="4"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C14" s="4"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C15" s="4"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:13" s="7" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="19">
+        <v>9</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="9">
+        <v>24000</v>
+      </c>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9">
+        <v>33392</v>
+      </c>
+      <c r="I11" s="9">
+        <v>16007</v>
+      </c>
+      <c r="J11" s="10">
+        <f>1-I11/H11</f>
+        <v>0.52063368471490179</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="L11" s="8"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:13" s="13" customFormat="1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="19">
+        <v>10</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="9">
+        <v>24000</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="9">
+        <v>33392</v>
+      </c>
+      <c r="I12" s="18">
+        <v>15992</v>
+      </c>
+      <c r="J12" s="10">
+        <f>1-I12/H12</f>
+        <v>0.52108289410637276</v>
+      </c>
+      <c r="K12" s="12"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="12"/>
+    </row>
+    <row r="13" spans="1:13" s="7" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="19">
+        <v>11</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="9">
+        <v>24000</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9">
+        <v>33392</v>
+      </c>
+      <c r="I13" s="16">
+        <v>1232</v>
+      </c>
+      <c r="J13" s="10">
+        <f>1-I13/H13</f>
+        <v>0.96310493531384767</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+    </row>
+    <row r="14" spans="1:13" s="7" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="19">
+        <v>12</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="9">
+        <v>24000</v>
+      </c>
+      <c r="G14" s="9"/>
+      <c r="H14" s="9">
+        <v>33392</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+    </row>
+    <row r="15" spans="1:13" ht="139" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="19">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="9">
+        <v>24000</v>
+      </c>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C16" s="4"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C17" s="4"/>
-      <c r="E17" s="2"/>
+      <c r="H15" s="9">
+        <v>33392</v>
+      </c>
+      <c r="I15" s="9">
+        <v>16007</v>
+      </c>
+      <c r="J15" s="10">
+        <f>1-I15/H15</f>
+        <v>0.52063368471490179</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="7" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="19">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="9">
+        <v>24000</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9">
+        <v>33392</v>
+      </c>
+      <c r="I16" s="9">
+        <v>4172</v>
+      </c>
+      <c r="J16" s="10">
+        <f>1-I16/H16</f>
+        <v>0.87505989458552946</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="L16" s="8"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D17" s="4"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C18" s="4"/>
-      <c r="E18" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D18" s="4"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C19" s="4"/>
-      <c r="E19" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="3"/>
+    </row>
+    <row r="19" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D19" s="4"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C20" s="4"/>
-      <c r="E20" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="3"/>
+    </row>
+    <row r="20" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D20" s="4"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C21" s="4"/>
-      <c r="E21" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D21" s="4"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C22" s="4"/>
-      <c r="E22" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="3"/>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D22" s="4"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C23" s="4"/>
-      <c r="E23" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="3"/>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D23" s="4"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C24" s="4"/>
-      <c r="E24" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="3"/>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D24" s="4"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C25" s="4"/>
-      <c r="E25" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="3"/>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D25" s="4"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C26" s="4"/>
-      <c r="E26" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D26" s="4"/>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C27" s="4"/>
-      <c r="E27" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D27" s="4"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C28" s="4"/>
-      <c r="E28" s="2"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="3"/>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D28" s="4"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C29" s="4"/>
-      <c r="E29" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="3"/>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D29" s="4"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C30" s="4"/>
-      <c r="E30" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="3"/>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D30" s="4"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C31" s="4"/>
-      <c r="E31" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="3"/>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D31" s="4"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C32" s="4"/>
-      <c r="E32" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="3"/>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D32" s="4"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C33" s="4"/>
-      <c r="E33" s="2"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="3"/>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D33" s="4"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C34" s="4"/>
-      <c r="E34" s="2"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="3"/>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D34" s="4"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C35" s="4"/>
-      <c r="E35" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="3"/>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D35" s="4"/>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C36" s="4"/>
-      <c r="E36" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="3"/>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D36" s="4"/>
       <c r="F36" s="2"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C37" s="4"/>
-      <c r="E37" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="3"/>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D37" s="4"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="C38" s="4"/>
-      <c r="E38" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="3"/>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D38" s="4"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="E39" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="3"/>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.2">
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="E40" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="3"/>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.2">
       <c r="F40" s="2"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
-      <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
-      <c r="I41" s="3"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="3"/>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="J41" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added one more experiment. still some doubts on strange behaviour
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D097FE-E1CE-7042-AD83-AA2894F0543C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088B96D1-B5B6-B849-954B-AC83D0EDC3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
   <si>
     <t>selected code</t>
   </si>
@@ -261,11 +261,47 @@
 I expect to have, since the two matrices are 15x15 and 15x16, three loops, of lenght (from the innermost one to the outermost) respectively 15, 16, 15 (this is understandable also from the optimized-intermediate.mlir). So if I fully unroll the innermost loop, I expect to have two loops of 15 and 16. But this is not the case, it seems that there are just two loops and that the innermost is repeated just two times.</t>
   </si>
   <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                           soda-opt \
+                                                             -soda-outline-bambu-code \
+                                                             -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                             -soda-generate-bambu-accelcode=no-aa \
+                                                             -convert-linalg-to-affine-loops \
+                                                             -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                             -mlir-print-ir-after-all \
+                                                             output/01searched-edited.mlir \
+                                                             -o output/04optimized.mlir \
+                                                             2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>Same number of cycles equal to the baseline AS expected.</t>
+  </si>
+  <si>
+    <t>Graph equal to the baseline.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                           soda-opt \
+                                                             -soda-outline-bambu-code \
+                                                             -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                             -soda-generate-bambu-accelcode=no-aa \
+                                                             -convert-linalg-to-affine-loops \
+                                                             --affine-loop-unroll="unroll-num-reps=1" \
+                                                             -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                             -mlir-print-ir-after-all \
+                                                             output/01searched-edited.mlir \
+                                                             -o output/04optimized.mlir \
+                                                             2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>I am now unrolling the innermost loop one time. In this way, the innermost number of iterations should decrease of 1. Instead more cycles, not coherent with my expectations. Changing from 1 to 15 does not affect the result, strange behaviour.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri (Corpo)"/>
       </rPr>
       <t>nb</t>
@@ -274,7 +310,7 @@
       <rPr>
         <b/>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -294,7 +330,7 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color rgb="FFFF0000"/>
+        <color theme="1"/>
         <rFont val="Calibri (Corpo)"/>
       </rPr>
       <t>red</t>
@@ -317,6 +353,7 @@
                                                              -soda-extract-arguments-to-xml=using-bare-ptr \
                                                              -soda-generate-bambu-accelcode=no-aa \
                                                              -convert-linalg-to-affine-loops \
+                                                             --affine-loop-unroll="unroll-full" \
                                                              -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
                                                              -mlir-print-ir-after-all \
                                                              output/01searched-edited.mlir \
@@ -324,34 +361,15 @@
                                                              2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
   </si>
   <si>
-    <t>Same number of cycles equal to the baseline AS expected.</t>
-  </si>
-  <si>
-    <t>Graph equal to the baseline.</t>
-  </si>
-  <si>
-    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
-                                                           soda-opt \
-                                                             -soda-outline-bambu-code \
-                                                             -soda-extract-arguments-to-xml=using-bare-ptr \
-                                                             -soda-generate-bambu-accelcode=no-aa \
-                                                             -convert-linalg-to-affine-loops \
-                                                             --affine-loop-unroll="unroll-num-reps=1" \
-                                                             -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
-                                                             -mlir-print-ir-after-all \
-                                                             output/01searched-edited.mlir \
-                                                             -o output/04optimized.mlir \
-                                                             2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
-  </si>
-  <si>
-    <t>I am now unrolling the innermost loop one time. In this way, the innermost number of iterations should go from 15 to 14. Instead more cycles, not coherent with my expectations. Changing from 1 to 15 does not affectthe result, strange behaviour.</t>
+    <t>This command has been tried in order to verify the correctness of these passes. Expected same result as full unroll 1, instead the outcome was of 36032 cycles, slightly different but again worst.
+It seems that, differently from what I was thinking, the no-aa option has not solved the strange behaviour. In the contrary, it seems that one of the command I am using (first three + last one) is affecting the result.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -374,22 +392,14 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <color theme="1"/>
+      <name val="Calibri (Corpo)"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri (Corpo)"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri (Corpo)"/>
     </font>
   </fonts>
@@ -425,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -465,9 +475,6 @@
     <xf numFmtId="3" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -477,14 +484,14 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -803,12 +810,12 @@
   <dimension ref="A1:M41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="17" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="20" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="49.1640625" customWidth="1"/>
     <col min="4" max="4" width="74.83203125" customWidth="1"/>
@@ -820,11 +827,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -852,7 +859,7 @@
       <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="19" t="s">
+      <c r="K2" s="18" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -863,7 +870,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="17">
+      <c r="A3" s="20">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -888,7 +895,7 @@
       <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="19" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -899,7 +906,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="17">
+      <c r="A4" s="20">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -924,7 +931,7 @@
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -935,7 +942,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="17">
+      <c r="A5" s="20">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -960,7 +967,7 @@
       <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="20" t="s">
+      <c r="K5" s="19" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -971,7 +978,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="17">
+      <c r="A6" s="20">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1005,7 +1012,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="17">
+      <c r="A7" s="20">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1036,7 +1043,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="17">
+      <c r="A8" s="20">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1067,7 +1074,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="17">
+      <c r="A9" s="20">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -1103,7 +1110,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21">
+      <c r="A10" s="20">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1136,7 +1143,7 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21">
+      <c r="A11" s="20">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1172,7 +1179,7 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" s="11" customFormat="1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21">
+      <c r="A12" s="20">
         <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1206,7 +1213,7 @@
       <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" s="6" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
+      <c r="A13" s="20">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1240,7 +1247,7 @@
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" s="6" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
+      <c r="A14" s="20">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1273,7 +1280,7 @@
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21">
+      <c r="A15" s="20">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -1304,7 +1311,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" s="6" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21">
+      <c r="A16" s="20">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1341,7 +1348,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D17" s="4"/>
       <c r="F17" s="2"/>
@@ -1351,17 +1358,17 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:13" s="6" customFormat="1" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="17">
+      <c r="A18" s="20">
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="8">
         <v>24000</v>
@@ -1378,7 +1385,7 @@
         <v>0</v>
       </c>
       <c r="K18" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
@@ -1391,19 +1398,19 @@
         <v>12</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G19" s="20"/>
-      <c r="H19" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I19" s="20">
+        <v>45</v>
+      </c>
+      <c r="F19" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G19" s="19"/>
+      <c r="H19" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I19" s="19">
         <v>36047</v>
       </c>
       <c r="J19" s="9">
@@ -1411,22 +1418,33 @@
         <v>-7.9510062290369055E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" s="7" customFormat="1" ht="238" x14ac:dyDescent="0.2">
       <c r="A20" s="22">
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F20" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I20" s="20"/>
-      <c r="J20" s="23"/>
+      <c r="C20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I20" s="19">
+        <v>36032</v>
+      </c>
+      <c r="J20" s="9">
+        <f>1-I20/H20</f>
+        <v>-7.906085289889786E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="22">
@@ -1435,15 +1453,15 @@
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I21" s="20"/>
-      <c r="J21" s="23"/>
+      <c r="F21" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I21" s="19"/>
+      <c r="J21" s="21"/>
     </row>
     <row r="22" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="22">
@@ -1452,15 +1470,15 @@
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I22" s="20"/>
-      <c r="J22" s="23"/>
+      <c r="F22" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I22" s="19"/>
+      <c r="J22" s="21"/>
     </row>
     <row r="23" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="22">
@@ -1469,15 +1487,15 @@
       <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I23" s="20"/>
-      <c r="J23" s="23"/>
+      <c r="F23" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I23" s="19"/>
+      <c r="J23" s="21"/>
     </row>
     <row r="24" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="22">
@@ -1486,15 +1504,15 @@
       <c r="B24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I24" s="20"/>
-      <c r="J24" s="23"/>
+      <c r="F24" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I24" s="19"/>
+      <c r="J24" s="21"/>
     </row>
     <row r="25" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="22">
@@ -1503,15 +1521,15 @@
       <c r="B25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I25" s="20"/>
-      <c r="J25" s="23"/>
+      <c r="F25" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I25" s="19"/>
+      <c r="J25" s="21"/>
     </row>
     <row r="26" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="22">
@@ -1520,15 +1538,15 @@
       <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I26" s="20"/>
-      <c r="J26" s="23"/>
+      <c r="F26" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I26" s="19"/>
+      <c r="J26" s="21"/>
     </row>
     <row r="27" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="22">
@@ -1537,15 +1555,15 @@
       <c r="B27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G27" s="20"/>
-      <c r="H27" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I27" s="20"/>
-      <c r="J27" s="23"/>
+      <c r="F27" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G27" s="19"/>
+      <c r="H27" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I27" s="19"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="22">
@@ -1554,15 +1572,15 @@
       <c r="B28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="20">
-        <v>24000</v>
-      </c>
-      <c r="G28" s="20"/>
-      <c r="H28" s="20">
-        <v>33392</v>
-      </c>
-      <c r="I28" s="20"/>
-      <c r="J28" s="23"/>
+      <c r="F28" s="19">
+        <v>24000</v>
+      </c>
+      <c r="G28" s="19"/>
+      <c r="H28" s="19">
+        <v>33392</v>
+      </c>
+      <c r="I28" s="19"/>
+      <c r="J28" s="21"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D29" s="4"/>

</xml_diff>

<commit_message>
added images and bash file to compile tex images and clear unwanted files
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088B96D1-B5B6-B849-954B-AC83D0EDC3FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F8753-41CF-BF42-A279-9D545ECEBC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -295,6 +295,24 @@
   </si>
   <si>
     <t>I am now unrolling the innermost loop one time. In this way, the innermost number of iterations should decrease of 1. Instead more cycles, not coherent with my expectations. Changing from 1 to 15 does not affect the result, strange behaviour.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                           soda-opt \
+                                                             -soda-outline-bambu-code \
+                                                             -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                             -soda-generate-bambu-accelcode=no-aa \
+                                                             -convert-linalg-to-affine-loops \
+                                                             --affine-loop-unroll="unroll-full" \
+                                                             -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                             -mlir-print-ir-after-all \
+                                                             output/01searched-edited.mlir \
+                                                             -o output/04optimized.mlir \
+                                                             2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>This command has been tried in order to verify the correctness of these passes. Expected same result as full unroll 1, instead the outcome was of 36032 cycles, slightly different but again worst.
+It seems that, differently from what I was thinking, the no-aa option has not solved the strange behaviour. In the contrary, it seems that one of the command I am using (first three + last one) is affecting the result.</t>
   </si>
   <si>
     <r>
@@ -325,15 +343,18 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> the reason why the loops were not correctly represented is because I was not using the no-aa parameter in the -soda-generate-bambu-accelcode=no-aa. From now on the tests will be more representetive, apparently kernel arguments marked with no alias, in combination with the lower-all-to-llvm were making some unwanted optimizations. This information make the </t>
+      <t xml:space="preserve"> the reason why the loops were not correctly represented </t>
     </r>
     <r>
       <rPr>
+        <i/>
         <sz val="12"/>
         <color theme="1"/>
-        <rFont val="Calibri (Corpo)"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
-      <t>red</t>
+      <t>should be</t>
     </r>
     <r>
       <rPr>
@@ -343,26 +364,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> experiments and their considerations not more valid.</t>
+      <t xml:space="preserve"> because I was not using the no-aa parameter in the -soda-generate-bambu-accelcode=no-aa. From now on the tests shoule be be more representetive, apparently kernel arguments marked with no alias, in combination with the lower-all-to-llvm were making some unwanted optimizations.</t>
     </r>
-  </si>
-  <si>
-    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
-                                                           soda-opt \
-                                                             -soda-outline-bambu-code \
-                                                             -soda-extract-arguments-to-xml=using-bare-ptr \
-                                                             -soda-generate-bambu-accelcode=no-aa \
-                                                             -convert-linalg-to-affine-loops \
-                                                             --affine-loop-unroll="unroll-full" \
-                                                             -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
-                                                             -mlir-print-ir-after-all \
-                                                             output/01searched-edited.mlir \
-                                                             -o output/04optimized.mlir \
-                                                             2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
-  </si>
-  <si>
-    <t>This command has been tried in order to verify the correctness of these passes. Expected same result as full unroll 1, instead the outcome was of 36032 cycles, slightly different but again worst.
-It seems that, differently from what I was thinking, the no-aa option has not solved the strange behaviour. In the contrary, it seems that one of the command I am using (first three + last one) is affecting the result.</t>
   </si>
 </sst>
 </file>
@@ -392,15 +395,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri (Corpo)"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri (Corpo)"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -476,9 +482,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -492,6 +495,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,13 +815,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
   <dimension ref="A1:M41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.5" style="20" customWidth="1"/>
+    <col min="1" max="1" width="5.5" style="19" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
     <col min="3" max="3" width="49.1640625" customWidth="1"/>
     <col min="4" max="4" width="74.83203125" customWidth="1"/>
@@ -827,11 +833,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
@@ -859,7 +865,7 @@
       <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="K2" s="17" t="s">
         <v>16</v>
       </c>
       <c r="L2" s="5" t="s">
@@ -870,7 +876,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
+      <c r="A3" s="19">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -895,7 +901,7 @@
       <c r="J3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="19" t="s">
+      <c r="K3" s="18" t="s">
         <v>21</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -906,7 +912,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A4" s="20">
+      <c r="A4" s="19">
         <v>2</v>
       </c>
       <c r="B4" t="s">
@@ -931,7 +937,7 @@
       <c r="J4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="18" t="s">
         <v>21</v>
       </c>
       <c r="L4" s="4" t="s">
@@ -942,7 +948,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
+      <c r="A5" s="19">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -967,7 +973,7 @@
       <c r="J5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="19" t="s">
+      <c r="K5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="L5" s="4" t="s">
@@ -978,7 +984,7 @@
       </c>
     </row>
     <row r="6" spans="1:13" ht="85" x14ac:dyDescent="0.2">
-      <c r="A6" s="20">
+      <c r="A6" s="19">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1012,7 +1018,7 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="20">
+      <c r="A7" s="19">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1043,7 +1049,7 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="20">
+      <c r="A8" s="19">
         <v>6</v>
       </c>
       <c r="B8" t="s">
@@ -1074,7 +1080,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A9" s="20">
+      <c r="A9" s="19">
         <v>7</v>
       </c>
       <c r="B9" t="s">
@@ -1110,7 +1116,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20">
+      <c r="A10" s="19">
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -1143,7 +1149,7 @@
       <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" s="6" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20">
+      <c r="A11" s="19">
         <v>9</v>
       </c>
       <c r="B11" s="6" t="s">
@@ -1179,7 +1185,7 @@
       <c r="M11" s="7"/>
     </row>
     <row r="12" spans="1:13" s="11" customFormat="1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20">
+      <c r="A12" s="19">
         <v>10</v>
       </c>
       <c r="B12" s="11" t="s">
@@ -1213,7 +1219,7 @@
       <c r="M12" s="10"/>
     </row>
     <row r="13" spans="1:13" s="6" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20">
+      <c r="A13" s="19">
         <v>11</v>
       </c>
       <c r="B13" s="6" t="s">
@@ -1247,7 +1253,7 @@
       <c r="M13" s="7"/>
     </row>
     <row r="14" spans="1:13" s="6" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20">
+      <c r="A14" s="19">
         <v>12</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -1280,7 +1286,7 @@
       <c r="M14" s="7"/>
     </row>
     <row r="15" spans="1:13" ht="139" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20">
+      <c r="A15" s="19">
         <v>13</v>
       </c>
       <c r="B15" s="6" t="s">
@@ -1311,7 +1317,7 @@
       </c>
     </row>
     <row r="16" spans="1:13" s="6" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20">
+      <c r="A16" s="19">
         <v>14</v>
       </c>
       <c r="B16" s="6" t="s">
@@ -1348,7 +1354,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D17" s="4"/>
       <c r="F17" s="2"/>
@@ -1358,7 +1364,7 @@
       <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:13" s="6" customFormat="1" ht="133" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20">
+      <c r="A18" s="19">
         <v>15</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -1391,7 +1397,7 @@
       <c r="M18" s="7"/>
     </row>
     <row r="19" spans="1:13" s="7" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="22">
+      <c r="A19" s="21">
         <v>16</v>
       </c>
       <c r="B19" s="7" t="s">
@@ -1403,14 +1409,14 @@
       <c r="D19" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I19" s="19">
+      <c r="F19" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I19" s="18">
         <v>36047</v>
       </c>
       <c r="J19" s="9">
@@ -1419,26 +1425,26 @@
       </c>
     </row>
     <row r="20" spans="1:13" s="7" customFormat="1" ht="238" x14ac:dyDescent="0.2">
-      <c r="A20" s="22">
+      <c r="A20" s="21">
         <v>17</v>
       </c>
       <c r="B20" s="7" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="F20" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I20" s="19">
+        <v>47</v>
+      </c>
+      <c r="F20" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I20" s="18">
         <v>36032</v>
       </c>
       <c r="J20" s="9">
@@ -1447,140 +1453,140 @@
       </c>
     </row>
     <row r="21" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="22">
+      <c r="A21" s="21">
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F21" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G21" s="19"/>
-      <c r="H21" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="21"/>
+      <c r="F21" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I21" s="18"/>
+      <c r="J21" s="20"/>
     </row>
     <row r="22" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="22">
+      <c r="A22" s="21">
         <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="21"/>
+      <c r="F22" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I22" s="18"/>
+      <c r="J22" s="20"/>
     </row>
     <row r="23" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="22">
+      <c r="A23" s="21">
         <v>20</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F23" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="21"/>
+      <c r="F23" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I23" s="18"/>
+      <c r="J23" s="20"/>
     </row>
     <row r="24" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="22">
+      <c r="A24" s="21">
         <v>21</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F24" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I24" s="19"/>
-      <c r="J24" s="21"/>
+      <c r="F24" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I24" s="18"/>
+      <c r="J24" s="20"/>
     </row>
     <row r="25" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A25" s="22">
+      <c r="A25" s="21">
         <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I25" s="19"/>
-      <c r="J25" s="21"/>
+      <c r="F25" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I25" s="18"/>
+      <c r="J25" s="20"/>
     </row>
     <row r="26" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="22">
+      <c r="A26" s="21">
         <v>23</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F26" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I26" s="19"/>
-      <c r="J26" s="21"/>
+      <c r="F26" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I26" s="18"/>
+      <c r="J26" s="20"/>
     </row>
     <row r="27" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="22">
+      <c r="A27" s="21">
         <v>24</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F27" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I27" s="19"/>
-      <c r="J27" s="21"/>
+      <c r="F27" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I27" s="18"/>
+      <c r="J27" s="20"/>
     </row>
     <row r="28" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="22">
+      <c r="A28" s="21">
         <v>25</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="19">
-        <v>24000</v>
-      </c>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19">
-        <v>33392</v>
-      </c>
-      <c r="I28" s="19"/>
-      <c r="J28" s="21"/>
+      <c r="F28" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I28" s="18"/>
+      <c r="J28" s="20"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D29" s="4"/>

</xml_diff>

<commit_message>
added correct way to perform experiments to spreadsheet. going to add more information soon
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46F8753-41CF-BF42-A279-9D545ECEBC11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F382C761-0421-6942-B41B-A431BD2F2452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="62">
   <si>
     <t>selected code</t>
   </si>
@@ -366,6 +366,97 @@
       </rPr>
       <t xml:space="preserve"> because I was not using the no-aa parameter in the -soda-generate-bambu-accelcode=no-aa. From now on the tests shoule be be more representetive, apparently kernel arguments marked with no alias, in combination with the lower-all-to-llvm were making some unwanted optimizations.</t>
     </r>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode=no-aa \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-tile \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>test to see if affine_loop tile has some impact on performances.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                  soda-opt \
+                                                  -soda-outline-bambu-code \
+                                                  -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                  -soda-generate-bambu-accelcode=no-aa \
+                                                  -convert-linalg-to-affine-loops \
+                                                  -affine-data-copy-generate \
+                                                  -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                  -mlir-print-ir-after-all \
+                                                  output/01searched-edited.mlir \
+                                                  -o output/04optimized.mlir \
+                                                  2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>test to see if affine_data_copy_generate has some impact on performances.</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Here there are only 2 loops. Strange because I did not perform the full unroll of the innermost loop.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-factor=2" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>This is the right command to unroll the loop as desired (in combination with changes made to Bambu command). I am going to unroll more and more and analyze memory and computation bottlenecks.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-factor=1" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>This is the right command to unroll the loop as desired (in combination with changes made to Bambu command). I am going to unroll more and more and analyze memory and computation bottlenecks. The unroll 1 has no effects on the loop, so it can be considered as a sort of baseline. Loop are slightly slower than baseline probably due to other some small optimizations in lower levels.</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-factor=3" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>In this case the unrolling behaves as expected, making three unrolls of the loop. In this way the innermost loop has no more 15 iterations but 5 (15 step 3).</t>
   </si>
 </sst>
 </file>
@@ -813,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
-  <dimension ref="A1:M41"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1423,8 +1514,11 @@
         <f>1-I19/H19</f>
         <v>-7.9510062290369055E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" s="7" customFormat="1" ht="238" x14ac:dyDescent="0.2">
+      <c r="K19" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="7" customFormat="1" ht="133" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
         <v>17</v>
       </c>
@@ -1452,13 +1546,22 @@
         <v>-7.906085289889786E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
         <v>18</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F21" s="18">
         <v>24000</v>
       </c>
@@ -1466,16 +1569,30 @@
       <c r="H21" s="18">
         <v>33392</v>
       </c>
-      <c r="I21" s="18"/>
-      <c r="J21" s="20"/>
-    </row>
-    <row r="22" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="I21" s="18">
+        <v>33392</v>
+      </c>
+      <c r="J21" s="9">
+        <f>1-I21/H21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" s="7" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>19</v>
       </c>
       <c r="B22" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C22" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="F22" s="18">
         <v>24000</v>
       </c>
@@ -1483,16 +1600,29 @@
       <c r="H22" s="18">
         <v>33392</v>
       </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="20"/>
-    </row>
-    <row r="23" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="I22" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="7" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21">
         <v>20</v>
       </c>
       <c r="B23" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C23" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>14</v>
+      </c>
       <c r="F23" s="18">
         <v>24000</v>
       </c>
@@ -1500,15 +1630,29 @@
       <c r="H23" s="18">
         <v>33392</v>
       </c>
-      <c r="I23" s="18"/>
-      <c r="J23" s="20"/>
-    </row>
-    <row r="24" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="I23" s="18">
+        <v>29792</v>
+      </c>
+      <c r="J23" s="9">
+        <f>1-I23/H23</f>
+        <v>0.10781025395304267</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="7" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21">
         <v>21</v>
       </c>
       <c r="B24" s="7" t="s">
         <v>12</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>14</v>
       </c>
       <c r="F24" s="18">
         <v>24000</v>
@@ -1517,16 +1661,27 @@
       <c r="H24" s="18">
         <v>33392</v>
       </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="20"/>
-    </row>
-    <row r="25" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="I24" s="18">
+        <v>23117</v>
+      </c>
+      <c r="J24" s="9">
+        <f>1-I24/H24</f>
+        <v>0.30770843315764251</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="7" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21">
         <v>22</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>12</v>
       </c>
+      <c r="C25" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="F25" s="18">
         <v>24000</v>
       </c>
@@ -1534,8 +1689,13 @@
       <c r="H25" s="18">
         <v>33392</v>
       </c>
-      <c r="I25" s="18"/>
-      <c r="J25" s="20"/>
+      <c r="I25" s="18">
+        <v>20192</v>
+      </c>
+      <c r="J25" s="9">
+        <f>1-I25/H25</f>
+        <v>0.39530426449448974</v>
+      </c>
     </row>
     <row r="26" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="21">
@@ -1588,13 +1748,19 @@
       <c r="I28" s="18"/>
       <c r="J28" s="20"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D29" s="4"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="3"/>
+    <row r="29" spans="1:13" s="7" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" s="18">
+        <v>24000</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18">
+        <v>33392</v>
+      </c>
+      <c r="I29" s="18"/>
+      <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D30" s="4"/>
@@ -1669,6 +1835,7 @@
       <c r="J38" s="3"/>
     </row>
     <row r="39" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="D39" s="4"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -1683,7 +1850,14 @@
       <c r="J40" s="3"/>
     </row>
     <row r="41" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2"/>
       <c r="J41" s="3"/>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.2">
+      <c r="J42" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
[R1] background update. TODO: graph feature vectors, swapping of the two parts, defining MLP, WL test, MLIR  and HLS
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB1757C-7728-E44F-AAEE-7EF6AFB6647B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB148D92-2A4E-784D-9F7C-29DC2DF5F22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="96">
   <si>
     <t>selected code</t>
   </si>
@@ -659,6 +659,24 @@
   AreaxTime                : 157106.540301
   Time                     : 3.599151
   Tot. Time                : 3.599151</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                                                soda-opt \
+                                                -soda-outline-bambu-code \
+                                                -soda-extract-arguments-to-xml=using-bare-ptr \
+                                                -soda-generate-bambu-accelcode \
+                                                -convert-linalg-to-affine-loops \
+                                                -affine-loop-unroll="unroll-full" \
+                                                -affine-loop-unroll="unroll-full" \
+                                                -lower-all-to-llvm=use-bare-ptr-memref-call-conv \
+                                                -mlir-print-ir-after-all \
+                                                output/01searched-edited.mlir \
+                                                -o output/04optimized.mlir \
+                                                2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>./bambu-ac_types-clang16.AppImage -v3 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4.5 --experimental-setup=BAMBU-BALANCED-MP --channels-number=32 --memory-allocation-policy=NO_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
   </si>
 </sst>
 </file>
@@ -1139,15 +1157,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
   <dimension ref="A1:O41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.5" style="20" customWidth="1"/>
-    <col min="2" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="4" width="24.1640625" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="49.1640625" customWidth="1"/>
     <col min="6" max="6" width="74.83203125" customWidth="1"/>
     <col min="7" max="8" width="20.83203125" customWidth="1"/>
@@ -1883,7 +1902,7 @@
         <v>29792</v>
       </c>
       <c r="L23" s="9">
-        <f t="shared" ref="L23:L38" si="0">1-K23/J23</f>
+        <f t="shared" ref="L23:L40" si="0">1-K23/J23</f>
         <v>0.10781025395304267</v>
       </c>
     </row>
@@ -2401,12 +2420,26 @@
       <c r="C40" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D40" s="7"/>
-      <c r="H40" s="2"/>
+      <c r="D40" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="H40" s="18">
+        <v>24000</v>
+      </c>
       <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="3"/>
+      <c r="J40" s="18">
+        <v>33392</v>
+      </c>
+      <c r="K40" s="8">
+        <v>813</v>
+      </c>
+      <c r="L40" s="9">
+        <f t="shared" si="0"/>
+        <v>0.97565285098227117</v>
+      </c>
       <c r="M40" s="7" t="s">
         <v>93</v>
       </c>

</xml_diff>

<commit_message>
added experiment about whole gcn with matmul 15, accelerated of a factor 400x
</commit_message>
<xml_diff>
--- a/experiments.xlsx
+++ b/experiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvlpr/PyCharmProjects/gnn-acceleration-master-thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB148D92-2A4E-784D-9F7C-29DC2DF5F22B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5140F427-7F16-D24E-B55A-AEAD52B435F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{FCB729E3-6DD5-D149-AD4C-4363E8FA0940}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="102">
   <si>
     <t>selected code</t>
   </si>
@@ -633,12 +633,6 @@
 cp: cannot stat '/tmp/appimage_extracted_5e2bed6bce9f374a789f6866ea86a2ff/usr/bambu_results_0.xml': No such file or directory</t>
   </si>
   <si>
-    <t>matmul15</t>
-  </si>
-  <si>
-    <t>Python time</t>
-  </si>
-  <si>
     <t>0.00010919570922851562 s</t>
   </si>
   <si>
@@ -677,6 +671,56 @@
   </si>
   <si>
     <t>./bambu-ac_types-clang16.AppImage -v3 --print-dot -lm --soft-float --compiler=I386_CLANG16 --device-name=xcu280-2Lfsvh2892-VVD --clock-period=4.5 --experimental-setup=BAMBU-BALANCED-MP --channels-number=32 --memory-allocation-policy=NO_BRAM --disable-function-proxy --generate-tb=forward_kernel_test.xml --simulate --evaluation --simulator=VERILATOR --top-fname=forward_kernel input.ll 2&gt;&amp;1 | tee bambu-log</t>
+  </si>
+  <si>
+    <t>gcn15</t>
+  </si>
+  <si>
+    <t>matmul15 (torch.mm 15x15 15x16)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Total cycles             : 46701 cycles
+  Number of executions     : 1
+  Average execution        : 46701 cycles
+  Slices                   : 9066
+  Luts                     : 36961
+  Power                    : 3.5419999999999998
+  Registers                : 29784
+  DSPs                     : 46
+  BRAMs                    : 0
+  Clock period             : 4.5
+  Design minimum period    : 4.4379999999999997
+  Design slack             : 0.062000000000000277
+  Frequency                : 225.3267237494367
+  AreaxTime                : 7660501.3035179991
+  Time                     : 207.25903799999998
+  Tot. Time                : 207.25903799999998</t>
+  </si>
+  <si>
+    <t>docker run -u $(id -u) -v $(pwd):/working_dir --rm agostini01/soda \
+                        soda-opt \
+                        -soda-outline-bambu-code \
+                        -soda-extract-arguments-to-xml=using-bare-ptr \
+                        -soda-generate-bambu-accelcode \
+                        -soda-opt-pipeline-for-bambu="no-buffer-trick use-bare-ptr-memref-call-conv number-of-full-unrolls=1" \
+                        -mlir-print-ir-after-all \
+                        output/01searched-edited.mlir \
+                        -o output/04optimized.mlir \
+                        2&gt;&amp;1 | cat &gt; output/05intermediate-optimized.mlir</t>
+  </si>
+  <si>
+    <t>bambu time [ns]</t>
+  </si>
+  <si>
+    <t>Python time [s]</t>
+  </si>
+  <si>
+    <t>207.25903799999998</t>
+  </si>
+  <si>
+    <t>Inference time: 0.00015425682067871094
+= 154,256 us 
+(torch profiler -&gt; 105us)</t>
   </si>
 </sst>
 </file>
@@ -771,7 +815,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -840,6 +884,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1155,10 +1211,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B727F5-D79F-8743-9663-6B9B41A2DF11}">
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1172,23 +1228,24 @@
     <col min="7" max="8" width="20.83203125" customWidth="1"/>
     <col min="9" max="9" width="1.6640625" customWidth="1"/>
     <col min="10" max="12" width="20.83203125" customWidth="1"/>
-    <col min="13" max="13" width="34.33203125" style="7" customWidth="1"/>
-    <col min="14" max="15" width="23.83203125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="20.83203125" style="29" customWidth="1"/>
+    <col min="14" max="14" width="34.33203125" style="7" customWidth="1"/>
+    <col min="15" max="16" width="23.83203125" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="M1" s="28" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="N1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="28"/>
       <c r="O1" s="28"/>
-    </row>
-    <row r="2" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P1" s="28"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>62</v>
@@ -1215,17 +1272,20 @@
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="M2" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="20">
         <v>1</v>
       </c>
@@ -1251,17 +1311,17 @@
       <c r="L3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="18" t="s">
         <v>21</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="20">
         <v>2</v>
       </c>
@@ -1287,17 +1347,17 @@
       <c r="L4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M4" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N4" s="4" t="s">
+      <c r="N4" s="18" t="s">
         <v>21</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+      <c r="P4" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="20">
         <v>3</v>
       </c>
@@ -1323,17 +1383,17 @@
       <c r="L5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="N5" s="4" t="s">
+      <c r="N5" s="18" t="s">
         <v>21</v>
       </c>
       <c r="O5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="85" x14ac:dyDescent="0.2">
+      <c r="P5" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="85" x14ac:dyDescent="0.2">
       <c r="A6" s="20">
         <v>4</v>
       </c>
@@ -1360,14 +1420,14 @@
         <f>1-K6/J6</f>
         <v>0</v>
       </c>
-      <c r="M6" s="7" t="s">
+      <c r="N6" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="N6" s="4" t="s">
+      <c r="O6" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="20">
         <v>5</v>
       </c>
@@ -1394,11 +1454,11 @@
         <f>1-K7/J7</f>
         <v>0.52108289410637276</v>
       </c>
-      <c r="M7" s="7" t="s">
+      <c r="N7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="20">
         <v>6</v>
       </c>
@@ -1425,11 +1485,11 @@
         <f>1-K8/J8</f>
         <v>0.96310493531384767</v>
       </c>
-      <c r="M8" s="7" t="s">
+      <c r="N8" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="20">
         <v>7</v>
       </c>
@@ -1455,17 +1515,17 @@
       <c r="L9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="M9" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="N9" s="4" t="s">
+      <c r="N9" s="7" t="s">
         <v>21</v>
       </c>
       <c r="O9" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P9" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20">
         <v>8</v>
       </c>
@@ -1497,10 +1557,11 @@
         <f>1-K10/J10</f>
         <v>0.52063368471490179</v>
       </c>
-      <c r="N10" s="7"/>
+      <c r="M10" s="31"/>
       <c r="O10" s="7"/>
-    </row>
-    <row r="11" spans="1:15" s="6" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" s="6" customFormat="1" ht="130" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20">
         <v>9</v>
       </c>
@@ -1530,13 +1591,14 @@
         <f>1-K11/J11</f>
         <v>0.52063368471490179</v>
       </c>
-      <c r="M11" s="7" t="s">
+      <c r="M11" s="31"/>
+      <c r="N11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="N11" s="7"/>
       <c r="O11" s="7"/>
-    </row>
-    <row r="12" spans="1:15" s="11" customFormat="1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="82" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20">
         <v>10</v>
       </c>
@@ -1566,11 +1628,12 @@
         <f>1-K12/J12</f>
         <v>0.52108289410637276</v>
       </c>
-      <c r="M12" s="10"/>
+      <c r="M12" s="31"/>
       <c r="N12" s="10"/>
       <c r="O12" s="10"/>
-    </row>
-    <row r="13" spans="1:15" s="6" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P12" s="10"/>
+    </row>
+    <row r="13" spans="1:16" s="6" customFormat="1" ht="94" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20">
         <v>11</v>
       </c>
@@ -1600,11 +1663,12 @@
         <f>1-K13/J13</f>
         <v>0.96310493531384767</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="31"/>
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
-    </row>
-    <row r="14" spans="1:15" s="6" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="1:16" s="6" customFormat="1" ht="102" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20">
         <v>12</v>
       </c>
@@ -1633,11 +1697,12 @@
       <c r="L14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="M14" s="7"/>
+      <c r="M14" s="31"/>
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
-    </row>
-    <row r="15" spans="1:15" ht="139" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="1:16" ht="139" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20">
         <v>13</v>
       </c>
@@ -1669,8 +1734,9 @@
         <f>1-K15/J15</f>
         <v>0.52063368471490179</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" s="6" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M15" s="31"/>
+    </row>
+    <row r="16" spans="1:16" s="6" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20">
         <v>14</v>
       </c>
@@ -1700,13 +1766,14 @@
         <f>1-K16/J16</f>
         <v>0.87505989458552946</v>
       </c>
-      <c r="M16" s="7" t="s">
+      <c r="M16" s="31"/>
+      <c r="N16" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="N16" s="7"/>
       <c r="O16" s="7"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B17" s="6" t="s">
         <v>49</v>
       </c>
@@ -1719,7 +1786,7 @@
       <c r="K17" s="2"/>
       <c r="L17" s="3"/>
     </row>
-    <row r="18" spans="1:15" s="6" customFormat="1" ht="133" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" s="6" customFormat="1" ht="133" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20">
         <v>15</v>
       </c>
@@ -1746,13 +1813,14 @@
         <f>1-K18/J18</f>
         <v>0</v>
       </c>
-      <c r="M18" s="7" t="s">
+      <c r="M18" s="31"/>
+      <c r="N18" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="N18" s="7"/>
       <c r="O18" s="7"/>
-    </row>
-    <row r="19" spans="1:15" s="7" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="1:16" s="7" customFormat="1" ht="162" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="21">
         <v>16</v>
       </c>
@@ -1779,11 +1847,12 @@
         <f>1-K19/J19</f>
         <v>-7.9510062290369055E-2</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="M19" s="31"/>
+      <c r="N19" s="7" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="1:15" s="7" customFormat="1" ht="133" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" s="7" customFormat="1" ht="133" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="21">
         <v>17</v>
       </c>
@@ -1810,8 +1879,9 @@
         <f>1-K20/J20</f>
         <v>-7.906085289889786E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M20" s="31"/>
+    </row>
+    <row r="21" spans="1:16" s="7" customFormat="1" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="21">
         <v>18</v>
       </c>
@@ -1841,8 +1911,9 @@
         <f>1-K21/J21</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:15" s="7" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M21" s="31"/>
+    </row>
+    <row r="22" spans="1:16" s="7" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="21">
         <v>19</v>
       </c>
@@ -1871,8 +1942,9 @@
       <c r="L22" s="19" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:15" s="7" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M22" s="32"/>
+    </row>
+    <row r="23" spans="1:16" s="7" customFormat="1" ht="124" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="21">
         <v>20</v>
       </c>
@@ -1905,8 +1977,9 @@
         <f t="shared" ref="L23:L40" si="0">1-K23/J23</f>
         <v>0.10781025395304267</v>
       </c>
-    </row>
-    <row r="24" spans="1:15" s="7" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M23" s="31"/>
+    </row>
+    <row r="24" spans="1:16" s="7" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21">
         <v>21</v>
       </c>
@@ -1939,8 +2012,9 @@
         <f t="shared" si="0"/>
         <v>0.30770843315764251</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" s="7" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M24" s="31"/>
+    </row>
+    <row r="25" spans="1:16" s="7" customFormat="1" ht="112" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21">
         <v>22</v>
       </c>
@@ -1970,8 +2044,9 @@
         <f t="shared" si="0"/>
         <v>0.39530426449448974</v>
       </c>
-    </row>
-    <row r="26" spans="1:15" s="7" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M25" s="31"/>
+    </row>
+    <row r="26" spans="1:16" s="7" customFormat="1" ht="96" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21">
         <v>23</v>
       </c>
@@ -1998,11 +2073,12 @@
         <f t="shared" si="0"/>
         <v>0.38811691423095351</v>
       </c>
-      <c r="M26" s="7" t="s">
+      <c r="M26" s="31"/>
+      <c r="N26" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="27" spans="1:15" s="7" customFormat="1" ht="92" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" s="7" customFormat="1" ht="92" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21">
         <v>24</v>
       </c>
@@ -2029,8 +2105,9 @@
         <f t="shared" si="0"/>
         <v>0.40114398658361283</v>
       </c>
-    </row>
-    <row r="28" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M27" s="31"/>
+    </row>
+    <row r="28" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21">
         <v>25</v>
       </c>
@@ -2060,11 +2137,12 @@
         <f t="shared" si="0"/>
         <v>0.51569238140872065</v>
       </c>
-      <c r="M28" s="7" t="s">
+      <c r="M28" s="31"/>
+      <c r="N28" s="7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21">
         <v>26</v>
       </c>
@@ -2094,11 +2172,12 @@
         <f t="shared" si="0"/>
         <v>0.52108289410637276</v>
       </c>
-      <c r="M29" s="7" t="s">
+      <c r="M29" s="31"/>
+      <c r="N29" s="7" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="30" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21">
         <v>27</v>
       </c>
@@ -2128,11 +2207,12 @@
         <f t="shared" si="0"/>
         <v>0.75646861523718256</v>
       </c>
-      <c r="M30" s="7" t="s">
+      <c r="M30" s="31"/>
+      <c r="N30" s="7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="31" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="21">
         <v>28</v>
       </c>
@@ -2162,11 +2242,12 @@
         <f t="shared" si="0"/>
         <v>0.75826545280306656</v>
       </c>
-      <c r="M31" s="7" t="s">
+      <c r="M31" s="31"/>
+      <c r="N31" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="32" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="21">
         <v>29</v>
       </c>
@@ -2196,11 +2277,12 @@
         <f t="shared" si="0"/>
         <v>0.87505989458552946</v>
       </c>
-      <c r="M32" s="7" t="s">
+      <c r="M32" s="31"/>
+      <c r="N32" s="7" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="33" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="21">
         <v>30</v>
       </c>
@@ -2230,11 +2312,12 @@
         <f t="shared" si="0"/>
         <v>0.87505989458552946</v>
       </c>
-      <c r="M33" s="7" t="s">
+      <c r="M33" s="31"/>
+      <c r="N33" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21">
         <v>30</v>
       </c>
@@ -2264,11 +2347,12 @@
         <f t="shared" si="0"/>
         <v>0.93255869669381886</v>
       </c>
-      <c r="M34" s="7" t="s">
+      <c r="M34" s="31"/>
+      <c r="N34" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="35" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="21">
         <v>31</v>
       </c>
@@ -2298,11 +2382,12 @@
         <f t="shared" si="0"/>
         <v>0.9298634403449928</v>
       </c>
-      <c r="M35" s="7" t="s">
+      <c r="M35" s="31"/>
+      <c r="N35" s="7" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="21">
         <v>32</v>
       </c>
@@ -2332,11 +2417,12 @@
         <f t="shared" si="0"/>
         <v>0.96891471011020602</v>
       </c>
-      <c r="M36" s="7" t="s">
+      <c r="M36" s="31"/>
+      <c r="N36" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="21">
         <v>33</v>
       </c>
@@ -2366,11 +2452,12 @@
         <f t="shared" si="0"/>
         <v>0.96310493531384767</v>
       </c>
-      <c r="M37" s="7" t="s">
+      <c r="M37" s="31"/>
+      <c r="N37" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" s="7" customFormat="1" ht="84" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="21">
         <v>34</v>
       </c>
@@ -2398,33 +2485,35 @@
         <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="39" spans="1:15" s="23" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M38" s="31"/>
+    </row>
+    <row r="39" spans="1:16" s="23" customFormat="1" ht="7" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="22"/>
       <c r="H39" s="24"/>
       <c r="I39" s="24"/>
       <c r="J39" s="24"/>
       <c r="K39" s="24"/>
       <c r="L39" s="25"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="27"/>
+      <c r="M39" s="33"/>
+      <c r="N39" s="26"/>
       <c r="O39" s="27"/>
-    </row>
-    <row r="40" spans="1:15" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P39" s="27"/>
+    </row>
+    <row r="40" spans="1:16" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20">
         <v>35</v>
       </c>
       <c r="B40" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C40" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="D40" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="F40" s="7" t="s">
         <v>92</v>
-      </c>
-      <c r="D40" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="F40" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="H40" s="18">
         <v>24000</v>
@@ -2440,18 +2529,48 @@
         <f t="shared" si="0"/>
         <v>0.97565285098227117</v>
       </c>
-      <c r="M40" s="7" t="s">
+      <c r="M40" s="31">
+        <v>3599151</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="92" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="20">
+        <v>36</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D41" s="7" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="F41" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="K41" s="18">
+        <v>46701</v>
+      </c>
       <c r="L41" s="3"/>
+      <c r="M41" s="34" t="s">
+        <v>100</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>96</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="N1:P1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="M41" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>